<commit_message>
software-STM: Add function to decode Alarm instruction
</commit_message>
<xml_diff>
--- a/software/documentation/instruction_set.xlsx
+++ b/software/documentation/instruction_set.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18528"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -9,17 +9,17 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16785" windowHeight="7500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16785" windowHeight="7500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027" fullCalcOnLoad="1"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="51">
   <si>
     <t>Instruction</t>
   </si>
@@ -163,12 +163,21 @@
   </si>
   <si>
     <t>enable</t>
+  </si>
+  <si>
+    <t>fetched</t>
+  </si>
+  <si>
+    <t>don't care</t>
+  </si>
+  <si>
+    <t>data</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$R-1C09]&quot; &quot;#,##0.00;[Red][$R-1C09]&quot;-&quot;#,##0.00"/>
   </numFmts>
@@ -448,7 +457,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -462,9 +471,45 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -477,52 +522,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
-    <cellStyle name="Heading" xfId="1"/>
-    <cellStyle name="Heading1" xfId="2"/>
+    <cellStyle name="Heading" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="Heading1" xfId="2" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
-    <cellStyle name="Result" xfId="3"/>
-    <cellStyle name="Result2" xfId="4"/>
+    <cellStyle name="Result" xfId="3" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Result2" xfId="4" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -833,11 +845,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:K20"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B3:N20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -848,69 +860,81 @@
     <col min="4" max="11" width="10.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:11" ht="15" thickBot="1"/>
-    <row r="4" spans="2:11">
-      <c r="B4" s="6" t="s">
+    <row r="3" spans="2:14" ht="15" thickBot="1"/>
+    <row r="4" spans="2:14">
+      <c r="B4" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="7"/>
-      <c r="I4" s="7"/>
-      <c r="J4" s="7"/>
-      <c r="K4" s="8"/>
-    </row>
-    <row r="5" spans="2:11">
-      <c r="B5" s="9" t="s">
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="19"/>
+      <c r="G4" s="19"/>
+      <c r="H4" s="19"/>
+      <c r="I4" s="19"/>
+      <c r="J4" s="19"/>
+      <c r="K4" s="20"/>
+    </row>
+    <row r="5" spans="2:14">
+      <c r="B5" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
-      <c r="I5" s="5"/>
-      <c r="J5" s="5"/>
-      <c r="K5" s="10"/>
-    </row>
-    <row r="6" spans="2:11" ht="15" thickBot="1">
-      <c r="B6" s="19"/>
-      <c r="C6" s="20"/>
-      <c r="D6" s="21" t="s">
+      <c r="E5" s="15"/>
+      <c r="F5" s="15"/>
+      <c r="G5" s="15"/>
+      <c r="H5" s="15"/>
+      <c r="I5" s="15"/>
+      <c r="J5" s="15"/>
+      <c r="K5" s="16"/>
+      <c r="M5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="N5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="2:14" ht="15" thickBot="1">
+      <c r="B6" s="22"/>
+      <c r="C6" s="17"/>
+      <c r="D6" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="21" t="s">
+      <c r="E6" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="F6" s="21" t="s">
+      <c r="F6" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="G6" s="21" t="s">
+      <c r="G6" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="H6" s="21" t="s">
+      <c r="H6" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="I6" s="21" t="s">
+      <c r="I6" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="J6" s="21" t="s">
+      <c r="J6" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="K6" s="22" t="s">
+      <c r="K6" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="2:11" ht="15" thickBot="1">
-      <c r="B7" s="11" t="s">
+      <c r="M6" s="23" t="s">
+        <v>33</v>
+      </c>
+      <c r="N6" s="23" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="2:14" ht="15" thickBot="1">
+      <c r="B7" s="10" t="s">
         <v>12</v>
       </c>
       <c r="C7" s="4" t="s">
@@ -937,12 +961,12 @@
       <c r="J7" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="K7" s="12" t="s">
+      <c r="K7" s="5" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="2:11" ht="15.75" thickTop="1" thickBot="1">
-      <c r="B8" s="13"/>
+    <row r="8" spans="2:14" ht="15.75" thickTop="1" thickBot="1">
+      <c r="B8" s="11"/>
       <c r="C8" s="2" t="s">
         <v>15</v>
       </c>
@@ -967,12 +991,12 @@
       <c r="J8" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="K8" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" spans="2:11">
-      <c r="B9" s="15" t="s">
+      <c r="K8" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="2:14">
+      <c r="B9" s="12" t="s">
         <v>41</v>
       </c>
       <c r="C9" s="3" t="s">
@@ -999,12 +1023,12 @@
       <c r="J9" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="K9" s="16" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="10" spans="2:11">
-      <c r="B10" s="17"/>
+      <c r="K9" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="2:14">
+      <c r="B10" s="13"/>
       <c r="C10" s="4" t="s">
         <v>36</v>
       </c>
@@ -1021,20 +1045,20 @@
         <v>30</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>17</v>
+        <v>47</v>
       </c>
       <c r="I10" s="4" t="s">
-        <v>17</v>
+        <v>48</v>
       </c>
       <c r="J10" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="K10" s="12" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="11" spans="2:11">
-      <c r="B11" s="17"/>
+      <c r="K10" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="2:14">
+      <c r="B11" s="13"/>
       <c r="C11" s="4" t="s">
         <v>37</v>
       </c>
@@ -1059,12 +1083,12 @@
       <c r="J11" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="K11" s="12" t="s">
+      <c r="K11" s="5" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="2:11">
-      <c r="B12" s="17"/>
+    <row r="12" spans="2:14">
+      <c r="B12" s="13"/>
       <c r="C12" s="4" t="s">
         <v>38</v>
       </c>
@@ -1089,12 +1113,12 @@
       <c r="J12" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="K12" s="12" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="13" spans="2:11">
-      <c r="B13" s="17"/>
+      <c r="K12" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="2:14">
+      <c r="B13" s="13"/>
       <c r="C13" s="4" t="s">
         <v>39</v>
       </c>
@@ -1111,20 +1135,20 @@
         <v>30</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>17</v>
+        <v>47</v>
       </c>
       <c r="I13" s="4" t="s">
-        <v>17</v>
+        <v>48</v>
       </c>
       <c r="J13" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="K13" s="12" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="14" spans="2:11" ht="15" thickBot="1">
-      <c r="B14" s="18"/>
+      <c r="K13" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="2:14" ht="15" thickBot="1">
+      <c r="B14" s="14"/>
       <c r="C14" s="2" t="s">
         <v>40</v>
       </c>
@@ -1149,11 +1173,11 @@
       <c r="J14" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="K14" s="14" t="s">
+      <c r="K14" s="6" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="2:11">
+    <row r="15" spans="2:14">
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
@@ -1165,7 +1189,7 @@
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
     </row>
-    <row r="16" spans="2:11">
+    <row r="16" spans="2:14">
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>

</xml_diff>

<commit_message>
software-STM: Alarm information is send to screen on screen request
</commit_message>
<xml_diff>
--- a/software/documentation/instruction_set.xlsx
+++ b/software/documentation/instruction_set.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="48">
   <si>
     <t>Instruction</t>
   </si>
@@ -102,9 +102,6 @@
     <t>second</t>
   </si>
   <si>
-    <t>day</t>
-  </si>
-  <si>
     <t>repeat</t>
   </si>
   <si>
@@ -135,15 +132,6 @@
     <t>set alarm label</t>
   </si>
   <si>
-    <t>get alarm time params</t>
-  </si>
-  <si>
-    <t>get alarm extra params</t>
-  </si>
-  <si>
-    <t>get alarm label</t>
-  </si>
-  <si>
     <t>Alarm</t>
   </si>
   <si>
@@ -153,9 +141,6 @@
     <t>0x14</t>
   </si>
   <si>
-    <t>0x15</t>
-  </si>
-  <si>
     <t>day/date sel</t>
   </si>
   <si>
@@ -172,6 +157,12 @@
   </si>
   <si>
     <t>data</t>
+  </si>
+  <si>
+    <t>get alarm min params</t>
+  </si>
+  <si>
+    <t>get alarm params</t>
   </si>
 </sst>
 </file>
@@ -211,7 +202,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="19">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -370,17 +361,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right style="medium">
         <color indexed="64"/>
@@ -388,15 +368,6 @@
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
       <bottom/>
       <diagonal/>
     </border>
@@ -457,7 +428,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -477,13 +448,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -492,24 +466,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -522,11 +487,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -849,7 +817,7 @@
   <dimension ref="B3:N20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -862,46 +830,46 @@
   <sheetData>
     <row r="3" spans="2:14" ht="15" thickBot="1"/>
     <row r="4" spans="2:14">
-      <c r="B4" s="18" t="s">
+      <c r="B4" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="19"/>
-      <c r="D4" s="19"/>
-      <c r="E4" s="19"/>
-      <c r="F4" s="19"/>
-      <c r="G4" s="19"/>
-      <c r="H4" s="19"/>
-      <c r="I4" s="19"/>
-      <c r="J4" s="19"/>
-      <c r="K4" s="20"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="17"/>
+      <c r="I4" s="17"/>
+      <c r="J4" s="17"/>
+      <c r="K4" s="18"/>
     </row>
     <row r="5" spans="2:14">
-      <c r="B5" s="21" t="s">
+      <c r="B5" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="15" t="s">
+      <c r="C5" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="15" t="s">
+      <c r="D5" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="E5" s="15"/>
-      <c r="F5" s="15"/>
-      <c r="G5" s="15"/>
-      <c r="H5" s="15"/>
-      <c r="I5" s="15"/>
-      <c r="J5" s="15"/>
-      <c r="K5" s="16"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="13"/>
+      <c r="H5" s="13"/>
+      <c r="I5" s="13"/>
+      <c r="J5" s="13"/>
+      <c r="K5" s="14"/>
       <c r="M5" s="1" t="s">
         <v>17</v>
       </c>
       <c r="N5" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="2:14" ht="15" thickBot="1">
-      <c r="B6" s="22"/>
-      <c r="C6" s="17"/>
+      <c r="B6" s="20"/>
+      <c r="C6" s="15"/>
       <c r="D6" s="8" t="s">
         <v>11</v>
       </c>
@@ -926,15 +894,15 @@
       <c r="K6" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="M6" s="23" t="s">
-        <v>33</v>
-      </c>
-      <c r="N6" s="23" t="s">
-        <v>50</v>
+      <c r="M6" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="N6" s="10" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="7" spans="2:14" ht="15" thickBot="1">
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="11" t="s">
         <v>12</v>
       </c>
       <c r="C7" s="4" t="s">
@@ -966,7 +934,7 @@
       </c>
     </row>
     <row r="8" spans="2:14" ht="15.75" thickTop="1" thickBot="1">
-      <c r="B8" s="11"/>
+      <c r="B8" s="12"/>
       <c r="C8" s="2" t="s">
         <v>15</v>
       </c>
@@ -996,11 +964,11 @@
       </c>
     </row>
     <row r="9" spans="2:14">
-      <c r="B9" s="12" t="s">
-        <v>41</v>
+      <c r="B9" s="21" t="s">
+        <v>37</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>18</v>
@@ -1015,40 +983,40 @@
         <v>25</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="J9" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K9" s="7" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="10" spans="2:14">
-      <c r="B10" s="13"/>
+      <c r="B10" s="22"/>
       <c r="C10" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E10" s="4" t="s">
         <v>19</v>
       </c>
       <c r="F10" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="G10" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="G10" s="4" t="s">
-        <v>30</v>
-      </c>
       <c r="H10" s="4" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="I10" s="4" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="J10" s="4" t="s">
         <v>17</v>
@@ -1058,87 +1026,87 @@
       </c>
     </row>
     <row r="11" spans="2:14">
-      <c r="B11" s="13"/>
+      <c r="B11" s="22"/>
       <c r="C11" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E11" s="4" t="s">
         <v>19</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I11" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="K11" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="12" spans="2:14">
-      <c r="B12" s="13"/>
-      <c r="C12" s="4" t="s">
+      <c r="B12" s="22"/>
+      <c r="C12" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D12" s="4" t="s">
         <v>38</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>42</v>
       </c>
       <c r="E12" s="4" t="s">
         <v>19</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="I12" s="4" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="K12" s="5" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="13" spans="2:14">
-      <c r="B13" s="13"/>
-      <c r="C13" s="4" t="s">
+      <c r="B13" s="22"/>
+      <c r="C13" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D13" s="4" t="s">
         <v>39</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>43</v>
       </c>
       <c r="E13" s="4" t="s">
         <v>19</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>47</v>
+        <v>17</v>
       </c>
       <c r="I13" s="4" t="s">
-        <v>48</v>
+        <v>17</v>
       </c>
       <c r="J13" s="4" t="s">
         <v>17</v>
@@ -1147,39 +1115,20 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="2:14" ht="15" thickBot="1">
-      <c r="B14" s="14"/>
-      <c r="C14" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="H14" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="I14" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="J14" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="K14" s="6" t="s">
-        <v>33</v>
-      </c>
+    <row r="14" spans="2:14">
+      <c r="B14" s="22"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="4"/>
+      <c r="J14" s="4"/>
+      <c r="K14" s="4"/>
     </row>
     <row r="15" spans="2:14">
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
+      <c r="B15" s="22"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
@@ -1252,11 +1201,11 @@
   </sheetData>
   <mergeCells count="6">
     <mergeCell ref="B7:B8"/>
-    <mergeCell ref="B9:B14"/>
     <mergeCell ref="D5:K5"/>
     <mergeCell ref="C5:C6"/>
     <mergeCell ref="B4:K4"/>
     <mergeCell ref="B5:B6"/>
+    <mergeCell ref="B9:B15"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0.39370078740157477" bottom="0.39370078740157477" header="0" footer="0"/>
   <headerFooter>

</xml_diff>

<commit_message>
software-STM: Alarm can receive its parameters from the screen
Bug: NPSC can't handle multiple instruction in buffer.
Look into nextion_bufferUpdate with the instruction and DMA buffer size
instruction not saved when DMA buffer size is different from the
instruction buffer size
</commit_message>
<xml_diff>
--- a/software/documentation/instruction_set.xlsx
+++ b/software/documentation/instruction_set.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="50">
   <si>
     <t>Instruction</t>
   </si>
@@ -163,6 +163,12 @@
   </si>
   <si>
     <t>get alarm params</t>
+  </si>
+  <si>
+    <t>set alarm enable</t>
+  </si>
+  <si>
+    <t>0x15</t>
   </si>
 </sst>
 </file>
@@ -817,7 +823,7 @@
   <dimension ref="B3:N20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1040,7 +1046,7 @@
         <v>33</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="H11" s="4" t="s">
         <v>32</v>
@@ -1057,38 +1063,38 @@
     </row>
     <row r="12" spans="2:14">
       <c r="B12" s="22"/>
-      <c r="C12" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="D12" s="4" t="s">
+      <c r="C12" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="D12" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="E12" s="4" t="s">
+      <c r="E12" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="F12" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G12" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="H12" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="I12" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="J12" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="K12" s="5" t="s">
+      <c r="F12" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="G12" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="H12" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="I12" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="J12" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="K12" s="10" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="13" spans="2:14">
       <c r="B13" s="22"/>
       <c r="C13" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D13" s="4" t="s">
         <v>39</v>
@@ -1097,7 +1103,7 @@
         <v>19</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="G13" s="4" t="s">
         <v>17</v>
@@ -1117,15 +1123,33 @@
     </row>
     <row r="14" spans="2:14">
       <c r="B14" s="22"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
-      <c r="I14" s="4"/>
-      <c r="J14" s="4"/>
-      <c r="K14" s="4"/>
+      <c r="C14" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I14" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="J14" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="K14" s="5" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="15" spans="2:14">
       <c r="B15" s="22"/>
@@ -1200,12 +1224,12 @@
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="B9:B15"/>
     <mergeCell ref="B7:B8"/>
     <mergeCell ref="D5:K5"/>
     <mergeCell ref="C5:C6"/>
     <mergeCell ref="B4:K4"/>
     <mergeCell ref="B5:B6"/>
-    <mergeCell ref="B9:B15"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0.39370078740157477" bottom="0.39370078740157477" header="0" footer="0"/>
   <headerFooter>

</xml_diff>